<commit_message>
Start reporting analytical part
</commit_message>
<xml_diff>
--- a/docs/results-convergence/convergence.xlsx
+++ b/docs/results-convergence/convergence.xlsx
@@ -351,11 +351,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72329856"/>
-        <c:axId val="72328320"/>
+        <c:axId val="88699648"/>
+        <c:axId val="88701184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72329856"/>
+        <c:axId val="88699648"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -363,27 +363,67 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Evaluation</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72328320"/>
+        <c:crossAx val="88701184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72328320"/>
+        <c:axId val="88701184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Quality</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72329856"/>
+        <c:crossAx val="88699648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -623,11 +663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61713408"/>
-        <c:axId val="71246592"/>
+        <c:axId val="88734720"/>
+        <c:axId val="90837760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61713408"/>
+        <c:axId val="88734720"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -635,27 +675,67 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Evaluation</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71246592"/>
+        <c:crossAx val="90837760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71246592"/>
+        <c:axId val="90837760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Quality</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61713408"/>
+        <c:crossAx val="88734720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -931,11 +1011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="54644096"/>
-        <c:axId val="72438912"/>
+        <c:axId val="181609984"/>
+        <c:axId val="181611520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54644096"/>
+        <c:axId val="181609984"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -943,27 +1023,67 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Evaluation</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72438912"/>
+        <c:crossAx val="181611520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72438912"/>
+        <c:axId val="181611520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Quality</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54644096"/>
+        <c:crossAx val="181609984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1384,7 +1504,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1770,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1974,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>